<commit_message>
Added WebDriver Manager. Added UpdateData method in Fillo
</commit_message>
<xml_diff>
--- a/src/main/java/datamanager/loginData.xlsx
+++ b/src/main/java/datamanager/loginData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simranraina\eclipse-workspace\UITest\src\main\java\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/s_raina_dxc_com/Documents/Desktop/UI_POM_Test_Framework/src/main/java/datamanager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCBB3C0-EA0F-4511-A864-D514D4A24617}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{8BCBB3C0-EA0F-4511-A864-D514D4A24617}" revIDLastSave="1" xr10:uidLastSave="{3A038D31-3845-4674-8FED-BC1DFA20CC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="login" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Email</t>
   </si>
@@ -40,12 +40,19 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,23 +87,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -113,10 +120,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -151,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,7 +210,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,7 +315,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -317,13 +324,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -333,7 +340,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -342,7 +349,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -351,7 +358,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,12 +368,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -397,7 +404,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -416,7 +423,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -428,21 +435,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="9.7265625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="21.453125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -452,8 +459,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -463,8 +473,11 @@
       <c r="C2">
         <v>1234</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -474,9 +487,10 @@
       <c r="C3">
         <v>12345</v>
       </c>
+      <c r="D3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed Drivers folders. Downgraded webdrivermanager
</commit_message>
<xml_diff>
--- a/src/main/java/datamanager/loginData.xlsx
+++ b/src/main/java/datamanager/loginData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Email</t>
   </si>
@@ -444,9 +444,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="9.7265625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="21.453125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="9.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>